<commit_message>
Add more benchmark results
</commit_message>
<xml_diff>
--- a/autoparallel-benchmarks/src/main/results/benchmark_results.xlsx
+++ b/autoparallel-benchmarks/src/main/results/benchmark_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="30">
   <si>
     <t>Mode</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>FFTBenchmark.serialFFTBenchmark</t>
+  </si>
+  <si>
+    <t>2^25</t>
+  </si>
+  <si>
+    <t>2048x2048</t>
+  </si>
+  <si>
+    <t>1536x1536</t>
+  </si>
+  <si>
+    <t>1024x1024</t>
+  </si>
+  <si>
+    <t>2560x2560</t>
+  </si>
+  <si>
+    <t>2^20</t>
+  </si>
+  <si>
+    <t>2^26</t>
+  </si>
+  <si>
+    <t>2^15</t>
   </si>
 </sst>
 </file>
@@ -129,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -137,6 +161,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -466,31 +493,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -514,7 +541,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>2000000000</v>
+      </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -537,7 +567,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -560,162 +591,790 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>1000000000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>200</v>
+      </c>
+      <c r="F8">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>2E-3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>500000000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>2E-3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>200</v>
+      </c>
+      <c r="F10">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>1E-3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>250000000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>2E-3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>2E-3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44.149000000000001</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16" s="3">
+        <v>148.631</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17" s="3">
         <v>16.297000000000001</v>
       </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9">
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17">
         <v>0.14799999999999999</v>
       </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>100</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18" s="3">
         <v>80.575000000000003</v>
       </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10">
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18">
         <v>1.5960000000000001</v>
       </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3">
+        <v>8.4760000000000009</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20" s="3">
+        <v>21.942</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>0.59</v>
+      </c>
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.7090000000000001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="I21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2.65</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C25" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>100</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25" s="3">
+        <v>50.293999999999997</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="I25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26" s="3">
+        <v>184.02199999999999</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>6.81</v>
+      </c>
+      <c r="I26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27" s="3">
         <v>18.899999999999999</v>
       </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13">
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27">
         <v>0.113</v>
       </c>
-      <c r="I13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28" s="3">
         <v>70.542000000000002</v>
       </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14">
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28">
         <v>0.38500000000000001</v>
       </c>
-      <c r="I14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+      <c r="I28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>500</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29" s="3">
+        <v>13.638</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+      <c r="F30" s="3">
+        <v>21.802</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="I30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>250</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31" s="3">
+        <v>10.558</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32" s="3">
+        <v>5.3949999999999996</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="I32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35" s="3">
+        <v>20.866</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <v>1.556</v>
+      </c>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36" s="3">
+        <v>23.003</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <v>2.137</v>
+      </c>
+      <c r="I36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37" s="3">
         <v>9.1440000000000001</v>
       </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17">
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37">
         <v>0.23400000000000001</v>
       </c>
-      <c r="I17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18">
-        <v>100</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38" s="3">
         <v>10.75</v>
       </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18">
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38">
         <v>0.23899999999999999</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>100</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41" s="3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42" s="3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I42" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="17">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -728,7 +1387,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -740,7 +1399,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>